<commit_message>
changing names and activating google sheet
</commit_message>
<xml_diff>
--- a/RPA Framework/Data/Config.xlsx
+++ b/RPA Framework/Data/Config.xlsx
@@ -167,15 +167,9 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
-    <t>https://www.handelsregister.de/rp_web/mask.do?Typ=n</t>
-  </si>
-  <si>
     <t>The wesite address</t>
   </si>
   <si>
@@ -201,6 +195,12 @@
   </si>
   <si>
     <t>.\Data\gsheet.p12</t>
+  </si>
+  <si>
+    <t>ResearchCenterQueue</t>
+  </si>
+  <si>
+    <t>https://www.handelsregister.de/rp_web/welcome.do</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -585,7 +585,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -605,45 +605,45 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1637,6 +1637,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
downloading, renaming, sending test docs with outlook
</commit_message>
<xml_diff>
--- a/RPA Framework/Data/Config.xlsx
+++ b/RPA Framework/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\poc\REFrameworkTest\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DE103260\Documents\botproject\ChatbotRPA\RPA Framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>https://www.handelsregister.de/rp_web/welcome.do</t>
+  </si>
+  <si>
+    <t>DownloadPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Administrator\Downloads\</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -646,7 +652,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>